<commit_message>
docs: documentação de requisitos e banco de dados.
</commit_message>
<xml_diff>
--- a/docs/1-CRONOGRAMA.xlsx
+++ b/docs/1-CRONOGRAMA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\pi_2_semestre\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304292A6-BF6E-4AA3-8941-67E7DBB22D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB121CA-9138-41B3-A332-7DE6FBEFEB25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cronograma" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>DATAS</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t>Escopo Sistema</t>
-  </si>
-  <si>
-    <t>working</t>
   </si>
   <si>
     <t>Requisitos</t>
@@ -136,14 +133,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA4C2F4"/>
-        <bgColor rgb="FFA4C2F4"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor rgb="FFF1C232"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF1C232"/>
-        <bgColor rgb="FFF1C232"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor rgb="FFA4C2F4"/>
       </patternFill>
     </fill>
   </fills>
@@ -211,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -231,24 +228,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -475,13 +469,13 @@
       <selection sqref="A1:I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -489,31 +483,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="I1" s="2">
         <v>45629</v>
       </c>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
@@ -537,10 +531,10 @@
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="12"/>
+      <c r="B2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="9"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -566,10 +560,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="5"/>
-      <c r="C3" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="12"/>
+      <c r="C3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="9"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
@@ -595,14 +589,14 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
-      <c r="I4" s="12"/>
+      <c r="I4" s="9"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
@@ -619,20 +613,20 @@
     </row>
     <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>2</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
@@ -646,18 +640,18 @@
       <c r="V5" s="6"/>
     </row>
     <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>7</v>
+      <c r="A6" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="F6" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="13"/>
-      <c r="H6" s="14"/>
+      <c r="F6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="12"/>
+      <c r="H6" s="13"/>
       <c r="I6" s="5"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
@@ -674,18 +668,18 @@
       <c r="V6" s="6"/>
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>8</v>
+      <c r="A7" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
-      <c r="F7" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="14"/>
+      <c r="F7" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="12"/>
+      <c r="H7" s="13"/>
       <c r="I7" s="5"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
@@ -702,18 +696,18 @@
       <c r="V7" s="6"/>
     </row>
     <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>9</v>
+      <c r="A8" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
-      <c r="F8" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" s="13"/>
-      <c r="H8" s="14"/>
+      <c r="F8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="12"/>
+      <c r="H8" s="13"/>
       <c r="I8" s="5"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
@@ -730,8 +724,8 @@
       <c r="V8" s="6"/>
     </row>
     <row r="9" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>10</v>
+      <c r="A9" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -739,7 +733,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="10" t="s">
         <v>2</v>
       </c>
       <c r="I9" s="5"/>
@@ -758,8 +752,8 @@
       <c r="V9" s="6"/>
     </row>
     <row r="10" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>11</v>
+      <c r="A10" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -768,7 +762,7 @@
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="10" t="s">
         <v>2</v>
       </c>
       <c r="J10" s="6"/>

</xml_diff>